<commit_message>
Add multiple DEK test
Add multiple DEK test
</commit_message>
<xml_diff>
--- a/NEO_Secure Mode_TW/Test case list.xlsx
+++ b/NEO_Secure Mode_TW/Test case list.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vivotech\regress\regression\regress_test\test_tree\NEO_Secure Mode_TW\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973F394E-0E8C-437C-A538-24C09E842FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="60" windowWidth="14490" windowHeight="9930"/>
+    <workbookView xWindow="6015" yWindow="1065" windowWidth="19275" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test case list" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="136">
   <si>
     <t>Test case no.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2534,12 +2540,36 @@
     <t>EGN35-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>EGN36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmd 81-0C/ 81-0D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EGN37</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS-5449, NSRED reader, cmd C7-3A w/ 01 (internal cmd)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EGN38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multiple DEK test, ex. KeySlot 00 = TDES KEY, KeySlot 03 = AES KEY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2677,7 +2707,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2696,16 +2726,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2717,10 +2741,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2728,9 +2749,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2746,13 +2764,21 @@
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2790,7 +2816,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2824,6 +2850,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2858,9 +2885,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3033,14 +3061,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="76.25" style="1" customWidth="1"/>
@@ -3049,7 +3077,7 @@
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3059,11 +3087,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5">
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -3075,35 +3103,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="94.5">
+    <row r="5" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -3117,7 +3145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="94.5">
+    <row r="6" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
@@ -3131,7 +3159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="94.5">
+    <row r="7" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -3145,7 +3173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="110.25">
+    <row r="8" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -3159,7 +3187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -3169,7 +3197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -3179,7 +3207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -3189,7 +3217,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -3199,7 +3227,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>69</v>
       </c>
@@ -3209,11 +3237,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="48">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="7" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -3223,11 +3251,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="7" t="s">
         <v>101</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -3237,8 +3265,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -3251,8 +3279,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="63.75">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -3265,18 +3293,18 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32.25">
-      <c r="A18" s="6"/>
+    <row r="18" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:4" ht="48">
-      <c r="A19" s="6" t="s">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>93</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -3289,8 +3317,8 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="94.5">
-      <c r="A20" s="6" t="s">
+    <row r="20" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -3303,7 +3331,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="63">
+    <row r="21" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>41</v>
       </c>
@@ -3317,7 +3345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="47.25">
+    <row r="22" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -3331,7 +3359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="47.25">
+    <row r="23" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
@@ -3345,8 +3373,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16.5">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3359,237 +3387,237 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="7" customFormat="1" ht="81.75">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:4" ht="81.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A30" s="6" t="s">
+    <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A32" s="6" t="s">
+    <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="7" customFormat="1" ht="66">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:4" ht="66" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48.75">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="32.25">
-      <c r="A36" s="11" t="s">
+    <row r="36" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="32.25">
-      <c r="A37" s="11" t="s">
+    <row r="37" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
         <v>113</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="48.75">
-      <c r="A38" s="11" t="s">
+    <row r="38" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>118</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="6" t="s">
         <v>117</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="16.5">
+    <row r="39" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="48">
-      <c r="A40" s="18" t="s">
+    <row r="40" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="14"/>
-    </row>
-    <row r="41" spans="1:4" ht="48">
-      <c r="A41" s="18" t="s">
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
         <v>115</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="14"/>
-    </row>
-    <row r="42" spans="1:4" s="7" customFormat="1" ht="16.5">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11" t="s">
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="11"/>
-      <c r="D42" s="10" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>59</v>
       </c>
@@ -3601,7 +3629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>60</v>
       </c>
@@ -3613,7 +3641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16.5">
+    <row r="45" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>62</v>
       </c>
@@ -3625,7 +3653,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>64</v>
       </c>
@@ -3637,7 +3665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>71</v>
       </c>
@@ -3649,19 +3677,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="94.5">
-      <c r="A48" s="15" t="s">
+    <row r="48" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="16" t="s">
+      <c r="C48" s="12"/>
+      <c r="D48" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>76</v>
       </c>
@@ -3673,7 +3701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="63.75">
+    <row r="50" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>78</v>
       </c>
@@ -3685,7 +3713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="96.75">
+    <row r="51" spans="1:4" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>81</v>
       </c>
@@ -3697,35 +3725,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="63">
+    <row r="52" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="47.25">
+    <row r="53" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C53" s="6" t="s">
         <v>84</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="128.25">
+    <row r="54" spans="1:4" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>108</v>
       </c>
@@ -3737,7 +3765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="63">
+    <row r="55" spans="1:4" ht="63" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>123</v>
       </c>
@@ -3749,7 +3777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="78.75">
+    <row r="56" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>125</v>
       </c>
@@ -3763,7 +3791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="78.75">
+    <row r="57" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>129</v>
       </c>
@@ -3774,6 +3802,42 @@
         <v>128</v>
       </c>
       <c r="D57" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>